<commit_message>
update avatar, resize image fixbug boxchat load history Add list user component Change layout boxchat
</commit_message>
<xml_diff>
--- a/document_tmp/demo_SEASOFT_laravel_nodejs_vujs.xlsx
+++ b/document_tmp/demo_SEASOFT_laravel_nodejs_vujs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Làm trang chat giống fb, list chat, khung chat</t>
   </si>
@@ -84,7 +84,14 @@
 https://laravel.com/docs/7.x/authentication</t>
   </si>
   <si>
-    <t>Show list user with vujs, call api</t>
+    <t>Làm chức năng chat room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chat được realtime
+Show được history chat:
+  + Cuộn lên top show history
+  + Cuộn lại chính xác vị trí ban đầu trước khi load history
+  + Viết api laravel load data: limit 10 item </t>
   </si>
 </sst>
 </file>
@@ -108,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +125,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -135,7 +148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -143,10 +156,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -504,13 +519,13 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="36.140625" customWidth="1"/>
     <col min="5" max="5" width="40.5703125" customWidth="1"/>
@@ -543,7 +558,7 @@
       <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -569,20 +584,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44075</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>